<commit_message>
refactoring into TotalPoints property for Ranking
</commit_message>
<xml_diff>
--- a/Data/Excel/Matches-Full-Data.xlsx
+++ b/Data/Excel/Matches-Full-Data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
   <si>
     <t>Novak Djokovic</t>
   </si>
@@ -433,7 +433,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -441,7 +441,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
@@ -449,7 +449,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
@@ -620,6 +620,26 @@
         <v>30</v>
       </c>
     </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>43123</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>